<commit_message>
recalculated ticks per meter because of new wheel tread
</commit_message>
<xml_diff>
--- a/Documents/00_Other/MiscCalcs.xlsx
+++ b/Documents/00_Other/MiscCalcs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Documents\School\YEAR 6\ModernMobility\Documents\00_Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F728BC3B-4166-4432-A0A9-BBDE90CCFF7B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,19 +63,19 @@
     <t>Pulses/Rev</t>
   </si>
   <si>
-    <t>Diameter</t>
-  </si>
-  <si>
     <t>meters/inch</t>
   </si>
   <si>
     <t>Ticks/Meter</t>
+  </si>
+  <si>
+    <t>Diameter (inches)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
@@ -459,11 +460,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -564,10 +565,10 @@
         <v>3.1415926535897931</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E12" s="4">
-        <v>4.75</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -580,7 +581,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1">
         <v>2.5399999999999999E-2</v>
@@ -594,11 +595,11 @@
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E17" s="1">
         <f>B13/(B12*E12*B14)</f>
-        <v>1350.8053189067621</v>
+        <v>1283.2650529614239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ticks per meter calculations
</commit_message>
<xml_diff>
--- a/Documents/00_Other/MiscCalcs.xlsx
+++ b/Documents/00_Other/MiscCalcs.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Documents\School\YEAR 6\ModernMobility\Documents\00_Other\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F728BC3B-4166-4432-A0A9-BBDE90CCFF7B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21820" windowHeight="9600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Constants</t>
   </si>
@@ -70,12 +64,18 @@
   </si>
   <si>
     <t>Diameter (inches)</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>left</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
@@ -453,29 +453,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1.77734375" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.81640625" customWidth="1"/>
+    <col min="4" max="4" width="21.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -485,7 +485,7 @@
       </c>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -499,7 +499,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -513,13 +513,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D5" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
@@ -528,7 +528,7 @@
         <v>111.24366103909065</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="28.75" x14ac:dyDescent="0.3">
       <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
@@ -537,7 +537,7 @@
         <v>7.7599655204737017</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="28.75" x14ac:dyDescent="0.3">
       <c r="D8" s="5" t="s">
         <v>8</v>
       </c>
@@ -546,7 +546,7 @@
         <v>1.7439118436031327</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -556,7 +556,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -568,18 +568,18 @@
         <v>14</v>
       </c>
       <c r="E12" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4.9859999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>509.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -587,19 +587,31 @@
         <v>2.5399999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>504.75</v>
+      </c>
       <c r="D16" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>508.5</v>
+      </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="1">
         <f>B13/(B12*E12*B14)</f>
-        <v>1283.2650529614239</v>
+        <v>1280.5847476133281</v>
       </c>
     </row>
   </sheetData>

</xml_diff>